<commit_message>
Clear mistake in code, where combustion and biomass was filtered instead of df_comb and df_biomass
</commit_message>
<xml_diff>
--- a/360_SLE_Topologie_Combustion.xlsx
+++ b/360_SLE_Topologie_Combustion.xlsx
@@ -543,13 +543,13 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>10351.7</v>
+        <v>10299.7</v>
       </c>
       <c r="D5" t="n">
-        <v>12139.2</v>
+        <v>12044.2</v>
       </c>
       <c r="E5" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6">
@@ -782,13 +782,13 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D4" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -891,13 +891,13 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>334.7</v>
+        <v>194.7</v>
       </c>
       <c r="D2" t="n">
-        <v>535.6</v>
+        <v>328.6</v>
       </c>
       <c r="E2" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -958,13 +958,13 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>9.050000000000001</v>
+        <v>8.75</v>
       </c>
       <c r="D2" t="n">
-        <v>8.6</v>
+        <v>7.9</v>
       </c>
       <c r="E2" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3">
@@ -1063,13 +1063,13 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D7" t="n">
-        <v>17.44</v>
+        <v>5.82</v>
       </c>
       <c r="E7" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8">
@@ -1126,13 +1126,13 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>3665.8</v>
+        <v>2925.8</v>
       </c>
       <c r="D10" t="n">
-        <v>5561.7</v>
+        <v>4657.2</v>
       </c>
       <c r="E10" t="n">
-        <v>58</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11">
@@ -1168,13 +1168,13 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>1139.6</v>
+        <v>1039.6</v>
       </c>
       <c r="D12" t="n">
-        <v>180</v>
+        <v>79</v>
       </c>
       <c r="E12" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -1361,13 +1361,13 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>20335.6</v>
+        <v>20314.1</v>
       </c>
       <c r="D8" t="n">
-        <v>22741.8</v>
+        <v>22719.3</v>
       </c>
       <c r="E8" t="n">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9">
@@ -1554,13 +1554,13 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>5.13</v>
+        <v>2.1</v>
       </c>
       <c r="D7" t="n">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E7" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8">
@@ -1596,13 +1596,13 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>2388.6</v>
+        <v>2348.4</v>
       </c>
       <c r="D9" t="n">
-        <v>3624.92</v>
+        <v>3541.82</v>
       </c>
       <c r="E9" t="n">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10">
@@ -1617,13 +1617,13 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>237.8</v>
+        <v>230.3</v>
       </c>
       <c r="D10" t="n">
         <v>5.3</v>
       </c>
       <c r="E10" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1637,7 +1637,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1726,13 +1726,13 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>47.2</v>
+        <v>42.5</v>
       </c>
       <c r="D4" t="n">
-        <v>95.5</v>
+        <v>83</v>
       </c>
       <c r="E4" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5">
@@ -1822,28 +1822,28 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Kondensationsmaschine mit Entnahme</t>
+          <t>Sonstige</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Rohbraunkohlen</t>
+          <t>Erdgas, Erdölgas</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>22800</v>
+        <v>16</v>
       </c>
       <c r="D9" t="n">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="E9" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Sonstige</t>
+          <t>Stirlingmotor</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -1852,10 +1852,10 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>16</v>
+        <v>19.2</v>
       </c>
       <c r="D10" t="n">
-        <v>23</v>
+        <v>44.2</v>
       </c>
       <c r="E10" t="n">
         <v>3</v>
@@ -1864,22 +1864,22 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Stirlingmotor</t>
+          <t>Verbrennungsmotor</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Erdgas, Erdölgas</t>
+          <t>Andere Gase</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>19.2</v>
+        <v>1791.5</v>
       </c>
       <c r="D11" t="n">
-        <v>44.2</v>
+        <v>2030.8</v>
       </c>
       <c r="E11" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12">
@@ -1890,17 +1890,17 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Andere Gase</t>
+          <t>Dieselkraftstoff</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>1791.5</v>
+        <v>676</v>
       </c>
       <c r="D12" t="n">
-        <v>2030.8</v>
+        <v>0</v>
       </c>
       <c r="E12" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
@@ -1911,17 +1911,17 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Dieselkraftstoff</t>
+          <t>Erdgas, Erdölgas</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>676</v>
+        <v>7307.77</v>
       </c>
       <c r="D13" t="n">
-        <v>0</v>
+        <v>11801.3</v>
       </c>
       <c r="E13" t="n">
-        <v>0</v>
+        <v>77</v>
       </c>
     </row>
     <row r="14">
@@ -1932,17 +1932,17 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Erdgas, Erdölgas</t>
+          <t>Flüssiggas</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>7546.77</v>
+        <v>5.5</v>
       </c>
       <c r="D14" t="n">
-        <v>11837.3</v>
+        <v>13.8</v>
       </c>
       <c r="E14" t="n">
-        <v>78</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15">
@@ -1953,37 +1953,16 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Flüssiggas</t>
+          <t>Heizöl, leicht</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>5.5</v>
+        <v>7054.5</v>
       </c>
       <c r="D15" t="n">
-        <v>13.8</v>
+        <v>30.9</v>
       </c>
       <c r="E15" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>Verbrennungsmotor</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>Heizöl, leicht</t>
-        </is>
-      </c>
-      <c r="C16" t="n">
-        <v>7054.5</v>
-      </c>
-      <c r="D16" t="n">
-        <v>30.9</v>
-      </c>
-      <c r="E16" t="n">
         <v>3</v>
       </c>
     </row>
@@ -2150,13 +2129,13 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D7" t="n">
-        <v>43.54</v>
+        <v>31.9</v>
       </c>
       <c r="E7" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8">
@@ -2213,13 +2192,13 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>194863.9</v>
+        <v>194611.9</v>
       </c>
       <c r="D10" t="n">
-        <v>4039266.2</v>
+        <v>4038804.2</v>
       </c>
       <c r="E10" t="n">
-        <v>93</v>
+        <v>83</v>
       </c>
     </row>
     <row r="11">
@@ -2255,13 +2234,13 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>1815</v>
+        <v>1565</v>
       </c>
       <c r="D12" t="n">
-        <v>41188</v>
+        <v>0</v>
       </c>
       <c r="E12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>